<commit_message>
updated figures and code for NOAA report
</commit_message>
<xml_diff>
--- a/photogrammetry/data/metadata/siteCoordinates.xlsx
+++ b/photogrammetry/data/metadata/siteCoordinates.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iancombs/Documents/GitHub/photogrammetryNOAA/photogrammetry/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB1FF6D-0672-7242-B482-F0845B5FBE21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="17240" yWindow="580" windowWidth="16360" windowHeight="17440" xr2:uid="{6629BE97-6F76-EA48-AE45-A736C90597F0}"/>
+    <workbookView xWindow="17235" yWindow="585" windowWidth="16365" windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Lat_Y</t>
   </si>
@@ -72,12 +66,21 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>IC-C3</t>
+  </si>
+  <si>
+    <t>IC-U3</t>
+  </si>
+  <si>
+    <t>IC-Z3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -415,23 +418,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324927E-CAF8-4F4E-AA26-4BA23EE9A8E0}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -445,7 +448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +462,7 @@
         <v>-81.484549999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -473,105 +476,148 @@
         <v>-81.485439999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>24.531089999999999</v>
+      </c>
+      <c r="D4">
+        <v>-81.485020000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>24.540700000000001</v>
-      </c>
-      <c r="D4">
-        <v>-81.443870000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5">
+        <v>24.540700000000001</v>
+      </c>
+      <c r="D5">
+        <v>-81.443870000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>24.54045</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>-81.445419999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>24.540469999999999</v>
+      </c>
+      <c r="D7">
+        <v>-81.444649999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>24.527660000000001</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>-81.497789999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>24.5274</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>-81.49897</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>24.53116</v>
-      </c>
-      <c r="D8">
-        <v>-81.484549999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>24.540700000000001</v>
-      </c>
-      <c r="D9">
-        <v>-81.443870000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
+        <v>24.527570000000001</v>
+      </c>
+      <c r="D10">
+        <v>-81.498429999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>24.53116</v>
+      </c>
+      <c r="D11">
+        <v>-81.484549999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>24.540700000000001</v>
+      </c>
+      <c r="D12">
+        <v>-81.443870000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
         <v>24.527660000000001</v>
       </c>
-      <c r="D10">
+      <c r="D13">
         <v>-81.497789999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>